<commit_message>
different lectures attempt different days
</commit_message>
<xml_diff>
--- a/CourseSchedule.xlsx
+++ b/CourseSchedule.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>Monday</t>
   </si>
@@ -32,159 +32,30 @@
     <t>08:00</t>
   </si>
   <si>
-    <t xml:space="preserve">MTH101
-MTH201
+    <t xml:space="preserve">CSE101-1
 </t>
   </si>
   <si>
-    <t xml:space="preserve">CHEM201
-MTH101
+    <t xml:space="preserve">CSE101-2
 </t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t xml:space="preserve">CHEM201
-MTH201
-</t>
-  </si>
-  <si>
     <t>09:15</t>
   </si>
   <si>
-    <t xml:space="preserve">MTH202
-ENG102
-MTH101
-MTH201
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTH301
-ENG202
-ENG301
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTH202
-PHY101
-ENG102
-ENG301
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTH301
-ENG202
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTH301
-PHY101
-ENG102
-ENG301
-</t>
-  </si>
-  <si>
     <t>10:30</t>
   </si>
   <si>
-    <t xml:space="preserve">CHEM101
-PHY301
-ENG102
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTH301
-ENG202
-CHEM101
-CSE202
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHEM101
-CSE202
-PHY101
-ENG301
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTH301
-ENG202
-BIO101
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHY101
-BIO101
-ENG301
-</t>
-  </si>
-  <si>
     <t>11:45</t>
   </si>
   <si>
-    <t xml:space="preserve">CHEM101
-PHY201-1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENG202
-BIO202
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHEM101
-CSE401
-ENG102
-BIO301
-PHY201-1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENG202
-CSE401
-CSE301
-BIO301
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIO202
-CSE401
-CSE301
-</t>
-  </si>
-  <si>
     <t>13:00</t>
   </si>
   <si>
-    <t xml:space="preserve">PHY201-2
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENG202
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE401
-CSE301
-PHY201-2
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE401
-CSE301
-</t>
-  </si>
-  <si>
     <t>14:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE301
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENG101
-</t>
   </si>
 </sst>
 </file>
@@ -263,10 +134,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -274,87 +145,87 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -363,13 +234,13 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADDED UNSCHEDULED COURSE FIXED STUFF
</commit_message>
<xml_diff>
--- a/CourseSchedule.xlsx
+++ b/CourseSchedule.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
   <si>
     <t>Monday</t>
   </si>
@@ -32,11 +32,7 @@
     <t>08:00</t>
   </si>
   <si>
-    <t xml:space="preserve">CSE101-1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE101-2
+    <t xml:space="preserve">CSE101
 </t>
   </si>
   <si>
@@ -140,107 +136,107 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actually fixed rescheduling now
</commit_message>
<xml_diff>
--- a/CourseSchedule.xlsx
+++ b/CourseSchedule.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>Monday</t>
   </si>
@@ -40,6 +40,10 @@
   </si>
   <si>
     <t>09:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTH202
+</t>
   </si>
   <si>
     <t>10:30</t>
@@ -144,13 +148,13 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -161,7 +165,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -181,7 +185,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -201,7 +205,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -221,7 +225,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
added queue to filereader
</commit_message>
<xml_diff>
--- a/CourseSchedule.xlsx
+++ b/CourseSchedule.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Monday</t>
   </si>
@@ -32,35 +32,39 @@
     <t>08:00</t>
   </si>
   <si>
-    <t xml:space="preserve">PHYS110
-PSYC301
-CMPS210
+    <t xml:space="preserve">CMPS210
 ENG205
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIST301
-MATH201
+PHYS110
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATH201
+HIST301
+ART202
 BUSN301
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSYC301
+PHYS110
+LANG202
+</t>
+  </si>
+  <si>
+    <t>09:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENG205
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENG205
+PHYS110
 </t>
   </si>
   <si>
     <t xml:space="preserve">PHYS110
 LANG202
-PSYC301
-</t>
-  </si>
-  <si>
-    <t>09:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENG205
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHYS110
-PSYC301
-ENG205
 </t>
   </si>
   <si>
@@ -71,28 +75,25 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">MATH201
+</t>
+  </si>
+  <si>
+    <t>11:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSYC301
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHEM202
-MATH201
-ART202
-</t>
-  </si>
-  <si>
-    <t>11:45</t>
+</t>
+  </si>
+  <si>
+    <t>13:00</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t xml:space="preserve">CHEM202
-ART202
-</t>
-  </si>
-  <si>
-    <t>13:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHEM202
-</t>
   </si>
   <si>
     <t>14:15</t>
@@ -200,87 +201,87 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>